<commit_message>
nrms models done + delete audio
</commit_message>
<xml_diff>
--- a/Machine Learning Workspace/WebService/webservice-input-output.xlsx
+++ b/Machine Learning Workspace/WebService/webservice-input-output.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adam\Documents\GitHub\Sustainable-AI-Challenge\Machine Learning Workspace\WebService\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3993DE04-D323-42DF-9EDE-CC2EFEA428BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA0F4257-BF34-46C6-AA08-A3ED3CFD1C43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ECECACC5-1A0D-4E8E-80ED-041977E7860F}"/>
+    <workbookView xWindow="28680" yWindow="2580" windowWidth="24240" windowHeight="13140" activeTab="2" xr2:uid="{ECECACC5-1A0D-4E8E-80ED-041977E7860F}"/>
   </bookViews>
   <sheets>
     <sheet name="toronto" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,6 @@
     <sheet name="bruce" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="46">
   <si>
     <t>Holiday</t>
   </si>
@@ -163,6 +162,15 @@
   </si>
   <si>
     <t>Bruce</t>
+  </si>
+  <si>
+    <t>AutoML_81bb32b6-9a40-4449-9f6f-ab701e0e2e47_31</t>
+  </si>
+  <si>
+    <t>AutoML_756310da-e42a-4f12-9229-d5b7d718f3f9</t>
+  </si>
+  <si>
+    <t>AutoML_a9ded8aa-5f46-4d7d-9f00-cc9ddd2f97bf_37</t>
   </si>
 </sst>
 </file>
@@ -555,8 +563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D76F524-CA96-4FA4-96DC-E038AE082C53}">
   <dimension ref="I3:W33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6:K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,6 +590,9 @@
       <c r="J4" t="s">
         <v>13</v>
       </c>
+      <c r="R4" t="s">
+        <v>43</v>
+      </c>
       <c r="S4" t="s">
         <v>37</v>
       </c>
@@ -661,7 +672,9 @@
       <c r="Q6">
         <v>4212</v>
       </c>
-      <c r="R6" s="6"/>
+      <c r="R6">
+        <v>3290.3887652841599</v>
+      </c>
       <c r="S6" s="7">
         <v>3845.9352147915101</v>
       </c>
@@ -672,7 +685,9 @@
         <v>4065.0373175271202</v>
       </c>
       <c r="V6" s="7"/>
-      <c r="W6" s="4"/>
+      <c r="W6" s="7">
+        <v>3820.20499967878</v>
+      </c>
     </row>
     <row r="7" spans="10:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="J7" s="2" t="s">
@@ -699,7 +714,9 @@
       <c r="Q7">
         <v>4083</v>
       </c>
-      <c r="R7" s="6"/>
+      <c r="R7">
+        <v>3238.2887598703601</v>
+      </c>
       <c r="S7" s="6">
         <v>3825.0230885209598</v>
       </c>
@@ -710,7 +727,9 @@
         <v>4065.0373175271202</v>
       </c>
       <c r="V7" s="6"/>
-      <c r="W7" s="5"/>
+      <c r="W7" s="6">
+        <v>3742.9094737222299</v>
+      </c>
     </row>
     <row r="8" spans="10:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="J8" s="2" t="s">
@@ -737,7 +756,9 @@
       <c r="Q8">
         <v>3997</v>
       </c>
-      <c r="R8" s="6"/>
+      <c r="R8">
+        <v>3241.79436967115</v>
+      </c>
       <c r="S8" s="6">
         <v>3595.0605804267602</v>
       </c>
@@ -748,7 +769,9 @@
         <v>4065.0373175271202</v>
       </c>
       <c r="V8" s="6"/>
-      <c r="W8" s="5"/>
+      <c r="W8" s="6">
+        <v>3699.8367336266301</v>
+      </c>
     </row>
     <row r="9" spans="10:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="J9" s="2" t="s">
@@ -775,7 +798,9 @@
       <c r="Q9">
         <v>3971</v>
       </c>
-      <c r="R9" s="6"/>
+      <c r="R9">
+        <v>3253.0403705685899</v>
+      </c>
       <c r="S9" s="6">
         <v>3576.5839571398501</v>
       </c>
@@ -786,7 +811,9 @@
         <v>4065.0373175271202</v>
       </c>
       <c r="V9" s="6"/>
-      <c r="W9" s="5"/>
+      <c r="W9" s="6">
+        <v>3745.9319280342902</v>
+      </c>
     </row>
     <row r="10" spans="10:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="J10" s="2" t="s">
@@ -813,7 +840,9 @@
       <c r="Q10">
         <v>4010</v>
       </c>
-      <c r="R10" s="6"/>
+      <c r="R10">
+        <v>3315.6568340706399</v>
+      </c>
       <c r="S10" s="6">
         <v>3651.0601694084098</v>
       </c>
@@ -824,7 +853,9 @@
         <v>4065.0373175271202</v>
       </c>
       <c r="V10" s="6"/>
-      <c r="W10" s="5"/>
+      <c r="W10" s="6">
+        <v>3756.4675588007299</v>
+      </c>
     </row>
     <row r="11" spans="10:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="J11" s="2" t="s">
@@ -851,7 +882,9 @@
       <c r="Q11">
         <v>4113</v>
       </c>
-      <c r="R11" s="6"/>
+      <c r="R11">
+        <v>3526.5225561775101</v>
+      </c>
       <c r="S11" s="6">
         <v>3731.2383402700798</v>
       </c>
@@ -862,7 +895,9 @@
         <v>4346.04800963041</v>
       </c>
       <c r="V11" s="6"/>
-      <c r="W11" s="5"/>
+      <c r="W11" s="6">
+        <v>3808.3145955854998</v>
+      </c>
     </row>
     <row r="12" spans="10:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="J12" s="2" t="s">
@@ -898,7 +933,9 @@
       </c>
       <c r="U12" s="6"/>
       <c r="V12" s="6"/>
-      <c r="W12" s="5"/>
+      <c r="W12" s="6">
+        <v>4128.4689949513604</v>
+      </c>
     </row>
     <row r="13" spans="10:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="J13" s="2" t="s">
@@ -934,7 +971,9 @@
       </c>
       <c r="U13" s="6"/>
       <c r="V13" s="6"/>
-      <c r="W13" s="5"/>
+      <c r="W13" s="6">
+        <v>4192.8950267595101</v>
+      </c>
     </row>
     <row r="14" spans="10:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="J14" s="2" t="s">
@@ -970,7 +1009,9 @@
       </c>
       <c r="U14" s="6"/>
       <c r="V14" s="6"/>
-      <c r="W14" s="5"/>
+      <c r="W14" s="7">
+        <v>4275.3458835909896</v>
+      </c>
     </row>
     <row r="15" spans="10:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="J15" s="2" t="s">
@@ -1006,7 +1047,9 @@
       </c>
       <c r="U15" s="6"/>
       <c r="V15" s="6"/>
-      <c r="W15" s="5"/>
+      <c r="W15" s="6">
+        <v>4537.5402871351898</v>
+      </c>
     </row>
     <row r="16" spans="10:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="J16" s="2" t="s">
@@ -1042,7 +1085,9 @@
       </c>
       <c r="U16" s="6"/>
       <c r="V16" s="6"/>
-      <c r="W16" s="5"/>
+      <c r="W16" s="6">
+        <v>4718.9127146525298</v>
+      </c>
     </row>
     <row r="17" spans="9:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="J17" s="2" t="s">
@@ -1078,7 +1123,9 @@
       </c>
       <c r="U17" s="6"/>
       <c r="V17" s="6"/>
-      <c r="W17" s="5"/>
+      <c r="W17" s="6">
+        <v>4878.4376221785396</v>
+      </c>
     </row>
     <row r="18" spans="9:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="J18" s="2" t="s">
@@ -1112,7 +1159,9 @@
       </c>
       <c r="U18" s="6"/>
       <c r="V18" s="6"/>
-      <c r="W18" s="5"/>
+      <c r="W18" s="6">
+        <v>4927.5790515091503</v>
+      </c>
     </row>
     <row r="19" spans="9:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="J19" s="2" t="s">
@@ -1146,7 +1195,9 @@
       </c>
       <c r="U19" s="6"/>
       <c r="V19" s="6"/>
-      <c r="W19" s="5"/>
+      <c r="W19" s="6">
+        <v>4958.2556706054902</v>
+      </c>
     </row>
     <row r="20" spans="9:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="J20" s="2" t="s">
@@ -1180,7 +1231,9 @@
       </c>
       <c r="U20" s="6"/>
       <c r="V20" s="6"/>
-      <c r="W20" s="5"/>
+      <c r="W20" s="6">
+        <v>4973.4895819912899</v>
+      </c>
     </row>
     <row r="21" spans="9:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="J21" s="2" t="s">
@@ -1214,7 +1267,9 @@
       </c>
       <c r="U21" s="6"/>
       <c r="V21" s="6"/>
-      <c r="W21" s="5"/>
+      <c r="W21" s="6">
+        <v>4953.1956190955098</v>
+      </c>
     </row>
     <row r="22" spans="9:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="J22" s="2" t="s">
@@ -1248,7 +1303,9 @@
       </c>
       <c r="U22" s="6"/>
       <c r="V22" s="6"/>
-      <c r="W22" s="5"/>
+      <c r="W22" s="6">
+        <v>5005.7743010412996</v>
+      </c>
     </row>
     <row r="23" spans="9:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="J23" s="2" t="s">
@@ -1282,7 +1339,9 @@
       </c>
       <c r="U23" s="6"/>
       <c r="V23" s="6"/>
-      <c r="W23" s="5"/>
+      <c r="W23" s="6">
+        <v>4997.9183271176098</v>
+      </c>
     </row>
     <row r="24" spans="9:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="J24" s="2" t="s">
@@ -1316,7 +1375,9 @@
       </c>
       <c r="U24" s="6"/>
       <c r="V24" s="6"/>
-      <c r="W24" s="5"/>
+      <c r="W24" s="6">
+        <v>4975.7937997561903</v>
+      </c>
     </row>
     <row r="25" spans="9:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="J25" s="2" t="s">
@@ -1350,7 +1411,9 @@
       </c>
       <c r="U25" s="6"/>
       <c r="V25" s="6"/>
-      <c r="W25" s="5"/>
+      <c r="W25" s="6">
+        <v>4963.9979589841796</v>
+      </c>
     </row>
     <row r="26" spans="9:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="J26" s="2" t="s">
@@ -1384,7 +1447,9 @@
       </c>
       <c r="U26" s="6"/>
       <c r="V26" s="6"/>
-      <c r="W26" s="5"/>
+      <c r="W26" s="6">
+        <v>4922.1928612105503</v>
+      </c>
     </row>
     <row r="27" spans="9:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="J27" s="2" t="s">
@@ -1418,7 +1483,9 @@
       </c>
       <c r="U27" s="6"/>
       <c r="V27" s="6"/>
-      <c r="W27" s="5"/>
+      <c r="W27" s="6">
+        <v>4936.5053247552996</v>
+      </c>
     </row>
     <row r="28" spans="9:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="J28" s="2" t="s">
@@ -1452,7 +1519,9 @@
       </c>
       <c r="U28" s="6"/>
       <c r="V28" s="6"/>
-      <c r="W28" s="5"/>
+      <c r="W28" s="6">
+        <v>4481.7182398412897</v>
+      </c>
     </row>
     <row r="29" spans="9:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="J29" s="2" t="s">
@@ -1486,7 +1555,13 @@
       </c>
       <c r="U29" s="6"/>
       <c r="V29" s="6"/>
-      <c r="W29" s="5"/>
+      <c r="W29" s="6">
+        <v>4303.2433347100005</v>
+      </c>
+    </row>
+    <row r="31" spans="9:23" x14ac:dyDescent="0.25">
+      <c r="J31" s="3"/>
+      <c r="R31" s="3"/>
     </row>
     <row r="32" spans="9:23" x14ac:dyDescent="0.25">
       <c r="I32" s="3"/>
@@ -1506,7 +1581,7 @@
   <dimension ref="E3:T32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G3:T5"/>
+      <selection activeCell="N30" sqref="N30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1604,6 +1679,9 @@
       <c r="N6" s="8">
         <v>709</v>
       </c>
+      <c r="O6" s="4">
+        <v>657.65162411475399</v>
+      </c>
       <c r="P6" s="4">
         <v>714.03094206617004</v>
       </c>
@@ -1636,6 +1714,9 @@
       <c r="N7" s="8">
         <v>690</v>
       </c>
+      <c r="O7" s="5">
+        <v>652.506964063429</v>
+      </c>
       <c r="P7" s="5">
         <v>699.50693251048801</v>
       </c>
@@ -1668,6 +1749,9 @@
       <c r="N8" s="8">
         <v>682</v>
       </c>
+      <c r="O8" s="5">
+        <v>641.55643438323398</v>
+      </c>
       <c r="P8" s="5">
         <v>698.44056186877503</v>
       </c>
@@ -1700,6 +1784,9 @@
       <c r="N9" s="8">
         <v>683</v>
       </c>
+      <c r="O9" s="5">
+        <v>647.91244323260696</v>
+      </c>
       <c r="P9" s="5">
         <v>696.24556328729204</v>
       </c>
@@ -1732,6 +1819,9 @@
       <c r="N10" s="8">
         <v>700</v>
       </c>
+      <c r="O10" s="5">
+        <v>677.312639607459</v>
+      </c>
       <c r="P10" s="5">
         <v>700.77154928760694</v>
       </c>
@@ -1764,6 +1854,9 @@
       <c r="N11" s="8">
         <v>730</v>
       </c>
+      <c r="O11" s="5">
+        <v>735.19097431752698</v>
+      </c>
       <c r="P11" s="5">
         <v>781.725430375575</v>
       </c>
@@ -2322,6 +2415,7 @@
     <row r="32" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E32" s="3"/>
       <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2330,14 +2424,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{185D8008-839C-47F4-A2B1-4F9CFB00FEB4}">
-  <dimension ref="F5:S7"/>
+  <dimension ref="F5:S35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView tabSelected="1" topLeftCell="F7" workbookViewId="0">
+      <selection activeCell="Q30" sqref="Q30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="6" max="6" width="27.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14.5703125" bestFit="1" customWidth="1"/>
@@ -2357,6 +2452,12 @@
       <c r="F6" t="s">
         <v>42</v>
       </c>
+      <c r="N6" t="s">
+        <v>45</v>
+      </c>
+      <c r="O6" t="s">
+        <v>44</v>
+      </c>
       <c r="Q6" t="s">
         <v>40</v>
       </c>
@@ -2404,6 +2505,766 @@
       <c r="S7" t="s">
         <v>17</v>
       </c>
+    </row>
+    <row r="8" spans="6:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>12.46</v>
+      </c>
+      <c r="I8">
+        <v>2.1</v>
+      </c>
+      <c r="J8">
+        <v>0.1</v>
+      </c>
+      <c r="K8">
+        <v>87</v>
+      </c>
+      <c r="L8" s="8">
+        <v>0</v>
+      </c>
+      <c r="M8" s="8">
+        <v>74</v>
+      </c>
+      <c r="N8">
+        <v>67.413971714951202</v>
+      </c>
+      <c r="O8" s="4">
+        <v>73.093543472835805</v>
+      </c>
+      <c r="P8" s="4">
+        <v>72.284167899482796</v>
+      </c>
+    </row>
+    <row r="9" spans="6:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" t="b">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>8.18</v>
+      </c>
+      <c r="I9">
+        <v>0.9</v>
+      </c>
+      <c r="J9">
+        <v>0.2</v>
+      </c>
+      <c r="K9">
+        <v>95</v>
+      </c>
+      <c r="L9" s="8">
+        <v>4</v>
+      </c>
+      <c r="M9" s="8">
+        <v>73</v>
+      </c>
+      <c r="N9">
+        <v>67.798828147214493</v>
+      </c>
+      <c r="O9" s="5">
+        <v>72.782795335966696</v>
+      </c>
+      <c r="P9" s="5">
+        <v>71.861100135209298</v>
+      </c>
+    </row>
+    <row r="10" spans="6:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>5.67</v>
+      </c>
+      <c r="I10">
+        <v>0.4</v>
+      </c>
+      <c r="J10">
+        <v>0.1</v>
+      </c>
+      <c r="K10">
+        <v>98</v>
+      </c>
+      <c r="L10" s="8">
+        <v>3</v>
+      </c>
+      <c r="M10" s="8">
+        <v>70</v>
+      </c>
+      <c r="N10">
+        <v>67.929761702497302</v>
+      </c>
+      <c r="O10" s="5">
+        <v>72.834033022160398</v>
+      </c>
+      <c r="P10" s="5">
+        <v>72.101609875475006</v>
+      </c>
+    </row>
+    <row r="11" spans="6:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" t="b">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>5.61</v>
+      </c>
+      <c r="I11">
+        <v>0.3</v>
+      </c>
+      <c r="J11">
+        <v>0.3</v>
+      </c>
+      <c r="K11">
+        <v>100</v>
+      </c>
+      <c r="L11" s="8">
+        <v>1</v>
+      </c>
+      <c r="M11" s="8">
+        <v>71</v>
+      </c>
+      <c r="N11">
+        <v>68.857644260292801</v>
+      </c>
+      <c r="O11" s="5">
+        <v>73.275596073871199</v>
+      </c>
+      <c r="P11" s="5">
+        <v>72.685457772374406</v>
+      </c>
+    </row>
+    <row r="12" spans="6:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" t="b">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>10.37</v>
+      </c>
+      <c r="I12">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="J12">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="K12">
+        <v>100</v>
+      </c>
+      <c r="L12" s="8">
+        <v>5</v>
+      </c>
+      <c r="M12" s="8">
+        <v>72</v>
+      </c>
+      <c r="N12">
+        <v>69.193422724356395</v>
+      </c>
+      <c r="O12" s="5">
+        <v>74.505976222369299</v>
+      </c>
+      <c r="P12" s="5">
+        <v>75.838931654377006</v>
+      </c>
+    </row>
+    <row r="13" spans="6:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>13.41</v>
+      </c>
+      <c r="I13">
+        <v>2.8</v>
+      </c>
+      <c r="J13">
+        <v>2.8</v>
+      </c>
+      <c r="K13">
+        <v>100</v>
+      </c>
+      <c r="L13" s="8">
+        <v>6</v>
+      </c>
+      <c r="M13" s="8">
+        <v>81</v>
+      </c>
+      <c r="N13">
+        <v>76.056016809119797</v>
+      </c>
+      <c r="O13" s="5">
+        <v>80.092317370738996</v>
+      </c>
+      <c r="P13" s="5">
+        <v>77.371626529193904</v>
+      </c>
+    </row>
+    <row r="14" spans="6:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>11.75</v>
+      </c>
+      <c r="I14">
+        <v>2.8</v>
+      </c>
+      <c r="J14">
+        <v>2.7</v>
+      </c>
+      <c r="K14">
+        <v>100</v>
+      </c>
+      <c r="L14" s="8">
+        <v>3</v>
+      </c>
+      <c r="M14" s="8">
+        <v>85</v>
+      </c>
+      <c r="O14" s="5">
+        <v>80.542493019297297</v>
+      </c>
+      <c r="P14" s="5">
+        <v>80.889789314021698</v>
+      </c>
+    </row>
+    <row r="15" spans="6:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>-1.1599999999999999</v>
+      </c>
+      <c r="I15">
+        <v>3.5</v>
+      </c>
+      <c r="J15">
+        <v>3.5</v>
+      </c>
+      <c r="K15">
+        <v>100</v>
+      </c>
+      <c r="L15" s="8">
+        <v>2</v>
+      </c>
+      <c r="M15" s="8">
+        <v>85</v>
+      </c>
+      <c r="O15" s="5">
+        <v>80.384831695456398</v>
+      </c>
+      <c r="P15" s="5">
+        <v>78.0797393384576</v>
+      </c>
+    </row>
+    <row r="16" spans="6:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G16" t="b">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>2.91</v>
+      </c>
+      <c r="I16">
+        <v>4.2</v>
+      </c>
+      <c r="J16">
+        <v>4.2</v>
+      </c>
+      <c r="K16">
+        <v>100</v>
+      </c>
+      <c r="L16" s="8">
+        <v>10</v>
+      </c>
+      <c r="M16" s="8">
+        <v>82</v>
+      </c>
+      <c r="O16" s="5">
+        <v>81.883284274690496</v>
+      </c>
+      <c r="P16" s="5">
+        <v>81.789484165995802</v>
+      </c>
+    </row>
+    <row r="17" spans="6:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" t="b">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>3.34</v>
+      </c>
+      <c r="I17">
+        <v>5.7</v>
+      </c>
+      <c r="J17">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="K17">
+        <v>95</v>
+      </c>
+      <c r="L17" s="8">
+        <v>8</v>
+      </c>
+      <c r="M17" s="8">
+        <v>79</v>
+      </c>
+      <c r="O17" s="5">
+        <v>82.363809932334902</v>
+      </c>
+      <c r="P17" s="5">
+        <v>82.150731403534607</v>
+      </c>
+    </row>
+    <row r="18" spans="6:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G18" t="b">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>4.82</v>
+      </c>
+      <c r="I18">
+        <v>7.8</v>
+      </c>
+      <c r="J18">
+        <v>5</v>
+      </c>
+      <c r="K18">
+        <v>82</v>
+      </c>
+      <c r="L18" s="8">
+        <v>9</v>
+      </c>
+      <c r="M18" s="8">
+        <v>77</v>
+      </c>
+      <c r="O18" s="5">
+        <v>82.414905418387505</v>
+      </c>
+      <c r="P18" s="5">
+        <v>79.209494165066801</v>
+      </c>
+    </row>
+    <row r="19" spans="6:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F19" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G19" t="b">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>13.63</v>
+      </c>
+      <c r="I19">
+        <v>8.4</v>
+      </c>
+      <c r="J19">
+        <v>4.7</v>
+      </c>
+      <c r="K19">
+        <v>77</v>
+      </c>
+      <c r="L19" s="8">
+        <v>7</v>
+      </c>
+      <c r="M19" s="8">
+        <v>75</v>
+      </c>
+      <c r="O19" s="5">
+        <v>83.143211666528799</v>
+      </c>
+      <c r="P19" s="5">
+        <v>78.289413208856004</v>
+      </c>
+    </row>
+    <row r="20" spans="6:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F20" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G20" t="b">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>12.73</v>
+      </c>
+      <c r="I20">
+        <v>8.1</v>
+      </c>
+      <c r="J20">
+        <v>3.5</v>
+      </c>
+      <c r="K20">
+        <v>73</v>
+      </c>
+      <c r="L20" s="8">
+        <v>12</v>
+      </c>
+      <c r="M20" s="8">
+        <v>75</v>
+      </c>
+      <c r="P20" s="5">
+        <v>77.751775956967094</v>
+      </c>
+    </row>
+    <row r="21" spans="6:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F21" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G21" t="b">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>12.08</v>
+      </c>
+      <c r="I21">
+        <v>8.1</v>
+      </c>
+      <c r="J21">
+        <v>3.5</v>
+      </c>
+      <c r="K21">
+        <v>72</v>
+      </c>
+      <c r="L21" s="8">
+        <v>11</v>
+      </c>
+      <c r="M21" s="8">
+        <v>77</v>
+      </c>
+      <c r="P21" s="5">
+        <v>77.428019850713895</v>
+      </c>
+    </row>
+    <row r="22" spans="6:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F22" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G22" t="b">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>10.89</v>
+      </c>
+      <c r="I22">
+        <v>7.4</v>
+      </c>
+      <c r="J22">
+        <v>2.9</v>
+      </c>
+      <c r="K22">
+        <v>73</v>
+      </c>
+      <c r="L22" s="8">
+        <v>7</v>
+      </c>
+      <c r="M22" s="8">
+        <v>78</v>
+      </c>
+      <c r="P22" s="5">
+        <v>77.285747110450004</v>
+      </c>
+    </row>
+    <row r="23" spans="6:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F23" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G23" t="b">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>14.03</v>
+      </c>
+      <c r="I23">
+        <v>8.9</v>
+      </c>
+      <c r="J23">
+        <v>3.6</v>
+      </c>
+      <c r="K23">
+        <v>69</v>
+      </c>
+      <c r="L23" s="8">
+        <v>4</v>
+      </c>
+      <c r="M23" s="8">
+        <v>80</v>
+      </c>
+      <c r="P23" s="5">
+        <v>79.502820516588898</v>
+      </c>
+    </row>
+    <row r="24" spans="6:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F24" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G24" t="b">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>24.05</v>
+      </c>
+      <c r="I24">
+        <v>6.3</v>
+      </c>
+      <c r="J24">
+        <v>3.2</v>
+      </c>
+      <c r="K24">
+        <v>81</v>
+      </c>
+      <c r="L24" s="8">
+        <v>7</v>
+      </c>
+      <c r="M24" s="8">
+        <v>86</v>
+      </c>
+      <c r="P24" s="5">
+        <v>80.955950363037203</v>
+      </c>
+    </row>
+    <row r="25" spans="6:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F25" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G25" t="b">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>13.19</v>
+      </c>
+      <c r="I25">
+        <v>5.2</v>
+      </c>
+      <c r="J25">
+        <v>3.1</v>
+      </c>
+      <c r="K25">
+        <v>86</v>
+      </c>
+      <c r="L25" s="8">
+        <v>4</v>
+      </c>
+      <c r="M25" s="8">
+        <v>85</v>
+      </c>
+      <c r="P25" s="5">
+        <v>81.2213891443471</v>
+      </c>
+    </row>
+    <row r="26" spans="6:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F26" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G26" t="b">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>13.31</v>
+      </c>
+      <c r="I26">
+        <v>4.5</v>
+      </c>
+      <c r="J26">
+        <v>3</v>
+      </c>
+      <c r="K26">
+        <v>90</v>
+      </c>
+      <c r="L26" s="8">
+        <v>10</v>
+      </c>
+      <c r="M26" s="8">
+        <v>81</v>
+      </c>
+      <c r="P26" s="5">
+        <v>79.503236296463996</v>
+      </c>
+    </row>
+    <row r="27" spans="6:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F27" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G27" t="b">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>12.69</v>
+      </c>
+      <c r="I27">
+        <v>2.5</v>
+      </c>
+      <c r="J27">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="K27">
+        <v>99</v>
+      </c>
+      <c r="L27" s="8">
+        <v>10</v>
+      </c>
+      <c r="M27" s="8">
+        <v>75</v>
+      </c>
+      <c r="P27" s="5">
+        <v>80.741919846063297</v>
+      </c>
+    </row>
+    <row r="28" spans="6:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F28" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G28" t="b">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>5.91</v>
+      </c>
+      <c r="I28">
+        <v>2.4</v>
+      </c>
+      <c r="J28">
+        <v>2.4</v>
+      </c>
+      <c r="K28">
+        <v>100</v>
+      </c>
+      <c r="L28" s="8">
+        <v>10</v>
+      </c>
+      <c r="M28" s="8">
+        <v>75</v>
+      </c>
+      <c r="P28" s="5">
+        <v>80.294196452817502</v>
+      </c>
+    </row>
+    <row r="29" spans="6:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F29" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G29" t="b">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>7.52</v>
+      </c>
+      <c r="I29">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="J29">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="K29">
+        <v>100</v>
+      </c>
+      <c r="L29" s="8">
+        <v>13</v>
+      </c>
+      <c r="M29" s="8">
+        <v>77</v>
+      </c>
+      <c r="P29" s="5">
+        <v>76.034855172271605</v>
+      </c>
+    </row>
+    <row r="30" spans="6:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F30" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G30" t="b">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>7.84</v>
+      </c>
+      <c r="I30">
+        <v>1.6</v>
+      </c>
+      <c r="J30">
+        <v>1.4</v>
+      </c>
+      <c r="K30">
+        <v>99</v>
+      </c>
+      <c r="L30" s="8">
+        <v>16</v>
+      </c>
+      <c r="M30" s="8">
+        <v>73</v>
+      </c>
+      <c r="P30" s="5">
+        <v>74.355691536289797</v>
+      </c>
+    </row>
+    <row r="31" spans="6:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F31" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G31" t="b">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>0.97</v>
+      </c>
+      <c r="I31">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J31">
+        <v>0.7</v>
+      </c>
+      <c r="K31">
+        <v>97</v>
+      </c>
+      <c r="L31" s="8">
+        <v>17</v>
+      </c>
+      <c r="M31" s="8">
+        <v>67</v>
+      </c>
+      <c r="P31" s="5">
+        <v>71.380864632141197</v>
+      </c>
+    </row>
+    <row r="32" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="L32" s="8"/>
+      <c r="M32" s="8"/>
+    </row>
+    <row r="33" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F33" s="3"/>
+    </row>
+    <row r="35" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F35" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>